<commit_message>
[20181025-2] add organization structure and customer / account / position / deal structure
</commit_message>
<xml_diff>
--- a/data_model/TABLE_ER_DIAGRAM.xlsx
+++ b/data_model/TABLE_ER_DIAGRAM.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816CE501-B9CE-4EFD-9813-1908CA0F4EF3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D438F99F-F27C-4AA2-8B51-28B4BF72F7CC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tables" sheetId="1" r:id="rId1"/>
+    <sheet name="BusinessObject" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
   <si>
     <t>CUSTOMER</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -105,12 +106,20 @@
     <t>SECURITIES_ISSUER</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>organization structure</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>customer / account / position / deal structure</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,8 +134,15 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -136,6 +152,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -167,10 +189,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -764,6 +788,1746 @@
         </a:prstGeom>
         <a:ln>
           <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>324223</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>126996</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>478116</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>97114</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="41" name="矩形: 圆角 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{073C7694-7889-4FC9-9CCE-9E3DE41AF2CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="324223" y="1202761"/>
+          <a:ext cx="5278717" cy="2838824"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>GLOBAL</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t> BUSINESS (PB)</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>642471</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>343647</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>59765</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="矩形: 圆角 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F2F6F34-3B89-4DAE-91FB-97C8C0011F9D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="642471" y="1703294"/>
+          <a:ext cx="4826000" cy="2121647"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>BOOKING</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t> ENTITY (HK)</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>358588</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>40341</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>212165</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>167341</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="39" name="矩形: 圆角 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5794D9B9-CC2F-440E-B921-3B0166EA1A70}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1016000" y="2550459"/>
+          <a:ext cx="1825812" cy="1023470"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>TEAM</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t> 2</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>388471</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>52294</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>29882</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="矩形: 圆角 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F38C465-D12E-408E-9812-B676BBC47466}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3018118" y="2562412"/>
+          <a:ext cx="2136588" cy="1023470"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>TEAM</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t> 1</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>830729</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>47064</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>112058</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>169208</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="矩形: 圆角 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C965914-A595-4695-8FF2-B5E1394BF95B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5955553" y="1302123"/>
+          <a:ext cx="5937623" cy="2811556"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>CUSTOMER (8000123456)</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>501650</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="矩形: 圆角 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{389DA465-6D45-425E-A8CF-430215A18BF7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5200650" y="1092200"/>
+          <a:ext cx="5238750" cy="2222500"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>CUSTOMER</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t> ACCOUNT (8000123456 - 0001)</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>920750</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="矩形: 圆角 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F1367D6-59F7-4530-B95C-3C2396662509}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5619750" y="1676400"/>
+          <a:ext cx="1320800" cy="482600"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>SHARE_POSITION</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>577850</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>577850</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="矩形: 圆角 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5C094B5-B50B-4CF1-A03F-D00A45AD9A5A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7118350" y="1676400"/>
+          <a:ext cx="1320800" cy="482600"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>BOND_POSITION</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>273050</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>273050</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="矩形: 圆角 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16804BDC-8E71-433C-8453-84830E504983}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8794750" y="1682750"/>
+          <a:ext cx="1320800" cy="482600"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>FUND_POSITION</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="矩形: 圆角 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B529F26-B020-478A-B8D9-5E2F4D6345AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5899150" y="2260600"/>
+          <a:ext cx="1035050" cy="260350"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>SHARE_DEAL</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="矩形: 圆角 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EA50C82-E496-42CD-B6B3-04267EB48D7A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5886450" y="2609850"/>
+          <a:ext cx="1035050" cy="260350"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>SHARE_DEAL</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>565150</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="矩形: 圆角 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{880AC0B3-9517-4279-8F43-A504AD878BC3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7391400" y="2260600"/>
+          <a:ext cx="1035050" cy="260350"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>BOND_DEAL</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="矩形: 圆角 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED4C43D5-AC97-476B-9F80-1C8294E2A639}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7378700" y="2609850"/>
+          <a:ext cx="1035050" cy="260350"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>BOND_DEAL</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>577850</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="矩形: 圆角 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6D09654-CACA-4EA9-9E28-F01D02A580DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9099550" y="2247900"/>
+          <a:ext cx="1035050" cy="260350"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>FUND_DEAL</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>565150</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="矩形: 圆角 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2E6B570-86F4-4865-9ED2-8ABC4FA6204B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9086850" y="2597150"/>
+          <a:ext cx="1035050" cy="260350"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>FUND_DEAL</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1041401</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>79374</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="连接符: 肘形 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96A81522-2CE0-46DF-9E07-A8BE87059D74}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="6" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="5710238" y="2201862"/>
+          <a:ext cx="219075" cy="158750"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1054100</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1060450</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="直接连接符 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60B38A6D-3E2B-4BC8-87F8-D9F9EAAF2460}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5753100" y="2190750"/>
+          <a:ext cx="6350" cy="546100"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="直接连接符 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{991A3243-AFE4-416A-B035-7307EB4CE651}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5727700" y="2381250"/>
+          <a:ext cx="184150" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1022350</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="直接连接符 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E3D22D8-53D6-4E9C-89FB-ED7219674375}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5721350" y="2705100"/>
+          <a:ext cx="184150" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>44450</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="直接连接符 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D1EC569-6A57-47D1-B56E-B49A5F7F9DEF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7245350" y="2203450"/>
+          <a:ext cx="6350" cy="546100"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="直接连接符 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1647966-8E65-4077-A192-BD52A87F4BC0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7219950" y="2393950"/>
+          <a:ext cx="184150" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>196850</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="直接连接符 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CA50DF4-AA43-4715-A652-86FBEE412886}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7213600" y="2717800"/>
+          <a:ext cx="184150" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="直接连接符 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4557A28-9AA3-492B-8455-B8143FBC380E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="8953500" y="2209800"/>
+          <a:ext cx="6350" cy="546100"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="直接连接符 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{546C598D-C0C4-4FDB-94DA-E07507084F2C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="8928100" y="2400300"/>
+          <a:ext cx="184150" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="直接连接符 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCFA2576-A8E5-4A7E-A774-24461940B5BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="8921750" y="2724150"/>
+          <a:ext cx="184150" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>836332</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>20543</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>417232</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>84044</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name="矩形: 圆角 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CA58DF5-4845-4EC7-91BC-C7A1DBA71BD5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4123391" y="2889249"/>
+          <a:ext cx="761253" cy="601383"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>RM 1</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>586068</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>13073</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>681318</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>76574</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="矩形: 圆角 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18856861-7EAD-4F2B-B041-6B4AFA4CA3A7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3215715" y="2881779"/>
+          <a:ext cx="752662" cy="601383"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>RM 2</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>417232</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>18302</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>521074</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>81803</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="矩形: 圆角 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{163749E7-22A4-4BEB-AE5F-169DF502FE0F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1732056" y="2887008"/>
+          <a:ext cx="761253" cy="601383"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>RM 3</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>417232</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>18489</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>830729</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>141941</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="43" name="连接符: 肘形 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF564CF3-ABAE-4F39-ADF2-18115AE7DF2C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="34" idx="3"/>
+          <a:endCxn id="33" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4884644" y="2707901"/>
+          <a:ext cx="1070909" cy="482040"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
           <a:tailEnd type="triangle"/>
         </a:ln>
       </xdr:spPr>
@@ -1052,8 +2816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -1231,4 +2995,38 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5B31F79-33CF-4700-9644-CBB0647F82BE}">
+  <dimension ref="C4:K4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="5" width="8.6640625" style="3"/>
+    <col min="6" max="6" width="15.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" style="3"/>
+    <col min="8" max="8" width="11.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.6640625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:11">
+      <c r="C4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
change the data model
</commit_message>
<xml_diff>
--- a/data_model/TABLE_ER_DIAGRAM.xlsx
+++ b/data_model/TABLE_ER_DIAGRAM.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D438F99F-F27C-4AA2-8B51-28B4BF72F7CC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22816F07-7D69-4521-B57F-F9B4C0568146}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
   <si>
     <t>CUSTOMER</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -47,19 +47,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>RM_CUSTOMER_MAP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>TEAM</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>TEAM_CODE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RM_TEAM_MAP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -112,6 +104,14 @@
   </si>
   <si>
     <t>customer / account / position / deal structure</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TEAM_CODE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOOKING_ENTITY</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -217,33 +217,33 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:colOff>14941</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>171824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>1494</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="连接符: 肘形 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{452AE7B1-C984-4E52-9BF6-5B923697E522}"/>
+        <xdr:cNvPr id="7" name="直接箭头连接符 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CC8350E-E1B5-4B78-AF71-F5409EFF933D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="2159000" y="641350"/>
-          <a:ext cx="1543050" cy="6350"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
+        <a:xfrm>
+          <a:off x="2427941" y="889000"/>
+          <a:ext cx="823259" cy="646953"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
           <a:avLst/>
         </a:prstGeom>
         <a:ln>
@@ -270,23 +270,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>660400</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1066800</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="5" name="直接箭头连接符 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45B537A2-FFC9-42CE-8C55-C232DA29FC38}"/>
+        <xdr:cNvPr id="11" name="直接箭头连接符 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F4062B6-B86D-4EA1-884D-2AB3F5A02B9F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -294,8 +294,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1320800" y="742950"/>
-          <a:ext cx="6350" cy="463550"/>
+          <a:off x="5016500" y="711200"/>
+          <a:ext cx="1714500" cy="977900"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -324,32 +324,32 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1536700</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1695450</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1079500</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="直接箭头连接符 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CC8350E-E1B5-4B78-AF71-F5409EFF933D}"/>
+        <xdr:cNvPr id="13" name="直接箭头连接符 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{078891A4-8366-4F04-810C-002FE20B2180}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="2451100" y="1524000"/>
-          <a:ext cx="1498600" cy="222250"/>
+        <a:xfrm>
+          <a:off x="4946650" y="882650"/>
+          <a:ext cx="1797050" cy="1771650"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -378,23 +378,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>717550</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>120650</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="8" name="直接箭头连接符 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46578364-6045-428F-BF73-8D99C38536B6}"/>
+        <xdr:cNvPr id="15" name="直接箭头连接符 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EA693E7-1C59-405F-B99C-930CE717FD3C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -402,8 +402,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4724400" y="1625600"/>
-          <a:ext cx="6350" cy="463550"/>
+          <a:off x="5124450" y="495300"/>
+          <a:ext cx="3829050" cy="901700"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -432,23 +432,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1568450</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="10" name="连接符: 肘形 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE5966FC-6778-465D-874E-1E065993588A}"/>
+        <xdr:cNvPr id="17" name="直接箭头连接符 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25C00EBA-1F00-4F7E-8513-0274D699DD6B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -456,10 +456,10 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2425700" y="2381250"/>
-          <a:ext cx="1555750" cy="57150"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
+          <a:off x="5080000" y="635000"/>
+          <a:ext cx="3810000" cy="1981200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
           <a:avLst/>
         </a:prstGeom>
         <a:ln>
@@ -486,23 +486,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1066800</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>593165</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>4482</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>605118</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>156882</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="11" name="直接箭头连接符 10">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F4062B6-B86D-4EA1-884D-2AB3F5A02B9F}"/>
+        <xdr:cNvPr id="20" name="直接箭头连接符 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{460B8CE4-7E77-4169-B979-A2B1EF70040F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -510,8 +510,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5016500" y="711200"/>
-          <a:ext cx="1714500" cy="977900"/>
+          <a:off x="7413812" y="3948953"/>
+          <a:ext cx="11953" cy="331694"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -540,32 +540,32 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1695450</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1079500</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>30629</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>29882</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>67235</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>22038</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="13" name="直接箭头连接符 12">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{078891A4-8366-4F04-810C-002FE20B2180}"/>
+        <xdr:cNvPr id="22" name="直接箭头连接符 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86DB45CA-9BC6-44CE-8120-1453ECFFAFFE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4946650" y="882650"/>
-          <a:ext cx="1797050" cy="1771650"/>
+        <a:xfrm flipV="1">
+          <a:off x="8300570" y="3974353"/>
+          <a:ext cx="694018" cy="530038"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -594,32 +594,32 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>120650</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1704041</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>82176</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>119155</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="15" name="直接箭头连接符 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EA693E7-1C59-405F-B99C-930CE717FD3C}"/>
+        <xdr:cNvPr id="16" name="直接箭头连接符 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE27E2BB-D8CF-4745-917B-98C42BD7787C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5124450" y="495300"/>
-          <a:ext cx="3829050" cy="901700"/>
+        <a:xfrm flipV="1">
+          <a:off x="2361453" y="1748118"/>
+          <a:ext cx="970429" cy="701861"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -648,140 +648,32 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>47812</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>622300</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:rowOff>97118</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>776941</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>100106</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="17" name="直接箭头连接符 16">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25C00EBA-1F00-4F7E-8513-0274D699DD6B}"/>
+        <xdr:cNvPr id="18" name="直接箭头连接符 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1241EF0-8DDE-44C0-9ED2-12C4A2064BCE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5080000" y="635000"/>
-          <a:ext cx="3810000" cy="1981200"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:headEnd type="triangle"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>593165</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>4482</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>605118</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>156882</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="20" name="直接箭头连接符 19">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{460B8CE4-7E77-4169-B979-A2B1EF70040F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7413812" y="3948953"/>
-          <a:ext cx="11953" cy="331694"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:headEnd type="triangle"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>30629</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>29882</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>67235</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>22038</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="22" name="直接箭头连接符 21">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86DB45CA-9BC6-44CE-8120-1453ECFFAFFE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="8300570" y="3974353"/>
-          <a:ext cx="694018" cy="530038"/>
+          <a:off x="2460812" y="635000"/>
+          <a:ext cx="729129" cy="2988"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2816,8 +2708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:I26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -2847,41 +2739,38 @@
       </c>
     </row>
     <row r="5" spans="2:9">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
       <c r="D5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="2:9">
-      <c r="B8" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="D8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="2:9">
-      <c r="B9" t="s">
-        <v>2</v>
-      </c>
       <c r="D9" t="s">
         <v>5</v>
       </c>
       <c r="G9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="2:9">
-      <c r="B10" t="s">
-        <v>5</v>
+      <c r="D10" t="s">
+        <v>21</v>
       </c>
       <c r="G10" t="s">
         <v>2</v>
@@ -2900,37 +2789,31 @@
     </row>
     <row r="12" spans="2:9">
       <c r="G12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="2:9">
       <c r="B13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="2:9">
       <c r="B14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="2:9">
-      <c r="D15" t="s">
-        <v>5</v>
+      <c r="B15" t="s">
+        <v>22</v>
       </c>
       <c r="G15" t="s">
         <v>2</v>
@@ -2949,44 +2832,44 @@
     </row>
     <row r="17" spans="7:9">
       <c r="G17" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I17" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="7:9">
       <c r="G20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="21" spans="7:9">
       <c r="G21" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I21" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="7:9">
       <c r="G22" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I22" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="7:9">
       <c r="G25" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="7:9">
       <c r="G26" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -3001,7 +2884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5B31F79-33CF-4700-9644-CBB0647F82BE}">
   <dimension ref="C4:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -3017,10 +2900,10 @@
   <sheetData>
     <row r="4" spans="3:11">
       <c r="C4" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>